<commit_message>
update api monitoring option
</commit_message>
<xml_diff>
--- a/checklist/checklist.xlsx
+++ b/checklist/checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="服务上线checklist" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>服务上线checklist</t>
   </si>
@@ -444,6 +444,12 @@
 1.日志查看
 2.容器exec
 3.本地主机端口映射集群容器端口（服务调试）</t>
+  </si>
+  <si>
+    <t>API监控</t>
+  </si>
+  <si>
+    <t>是否存在需要监控的api，如存在请填写完整的url和参数</t>
   </si>
   <si>
     <t>串讲纪要</t>
@@ -538,8 +544,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -573,15 +579,68 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -595,52 +654,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -654,19 +676,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -678,39 +692,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -731,25 +737,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,13 +881,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,139 +911,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,10 +985,41 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1003,15 +1040,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1023,30 +1051,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1068,9 +1072,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1082,10 +1088,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1094,133 +1100,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1603,10 +1609,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1792,7 +1798,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1810,21 +1816,30 @@
         <v>42</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" ht="25" customHeight="1" spans="1:3">
-      <c r="A24" s="7" t="s">
+    <row r="23" ht="16.5" spans="1:3">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" ht="25" customHeight="1" spans="1:3">
+      <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>